<commit_message>
Extent Reports and pom.xml build
</commit_message>
<xml_diff>
--- a/com.inetBanking/TestData/TestData.xlsx
+++ b/com.inetBanking/TestData/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasan\eclipse-workspace\com.inetBanking\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasan\git\inetBanking_hybrid_Framework\com.inetBanking\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF246B33-B43A-4FC2-870C-3B6DDCF9A520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375FCB3A-849A-4CDD-BB7B-72ABE6A23E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -37,12 +37,6 @@
     <t>ExpTitle</t>
   </si>
   <si>
-    <t>mngr511285</t>
-  </si>
-  <si>
-    <t>YpepUne</t>
-  </si>
-  <si>
     <t>Guru99 Bank Manager HomePage</t>
   </si>
   <si>
@@ -140,13 +134,18 @@
   </si>
   <si>
     <t>77572</t>
+  </si>
+  <si>
+    <t>mngr516939</t>
+  </si>
+  <si>
+    <t>dyhAmUd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -500,15 +499,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.77734375"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.5546875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="58.77734375"/>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.3">
@@ -524,13 +523,13 @@
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -543,151 +542,151 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74AE6F5-C10E-429A-AF4B-385CF2BCC0F0}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.33203125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.33203125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.77734375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.0"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="19.33203125"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3">
         <v>44308</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C3" s="3">
         <v>44582</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
         <v>44310</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>